<commit_message>
add extra columns to show info on 2 bachelor levels
</commit_message>
<xml_diff>
--- a/application/modules/stat/templates/report5.xlsx
+++ b/application/modules/stat/templates/report5.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\MyGitHub\cont_stat\application\modules\stat\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="21840" windowHeight="12645"/>
+    <workbookView xWindow="244" yWindow="122" windowWidth="21844" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Рух контингенту" sheetId="2" r:id="rId1"/>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>випуск</t>
   </si>
@@ -78,12 +83,18 @@
   <si>
     <t>%s контингенту %sстудентів вищих навчальних медичних закладів 3-4 рівнів акредитації МОЗ України, 
 %sза %s, на %s рік</t>
+  </si>
+  <si>
+    <t>молодших бакалаврів</t>
+  </si>
+  <si>
+    <t>молодших фахових бакалаврів</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -192,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -218,6 +229,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -253,7 +267,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -261,14 +275,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -306,9 +323,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -343,7 +360,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -378,7 +395,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -555,74 +572,86 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1"/>
-    <col min="3" max="14" width="6.7109375" customWidth="1"/>
-    <col min="15" max="17" width="6.7109375" style="3" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" customWidth="1"/>
-    <col min="19" max="20" width="6.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="29.59765625" customWidth="1"/>
+    <col min="3" max="7" width="6.69921875" customWidth="1"/>
+    <col min="8" max="9" width="6.69921875" style="7" customWidth="1"/>
+    <col min="10" max="14" width="6.69921875" customWidth="1"/>
+    <col min="15" max="16" width="6.69921875" style="7" customWidth="1"/>
+    <col min="17" max="18" width="6.69921875" customWidth="1"/>
+    <col min="19" max="21" width="6.69921875" style="3" customWidth="1"/>
+    <col min="22" max="22" width="6.69921875" customWidth="1"/>
+    <col min="23" max="24" width="6.69921875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
     </row>
-    <row r="2" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
+    <row r="2" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
     </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:24" ht="14.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="20" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -645,11 +674,15 @@
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
     </row>
-    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="9" t="s">
+    <row r="5" spans="1:24" ht="14.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="10" t="s">
@@ -659,39 +692,43 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="S5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="16" t="s">
+      <c r="T5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="16" t="s">
+      <c r="U5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="R5" s="16" t="s">
+      <c r="V5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="S5" s="11" t="s">
+      <c r="W5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="X5" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="9"/>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6" s="18"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="10" t="s">
         <v>1</v>
       </c>
@@ -701,27 +738,31 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="L6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
       <c r="M6" s="10"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="9"/>
+    <row r="7" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="10"/>
       <c r="E7" s="8" t="s">
         <v>10</v>
@@ -732,31 +773,43 @@
       <c r="G7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="10"/>
+      <c r="I7" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="J7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="M7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="N7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="O7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
+      <c r="P7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -772,37 +825,41 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1">
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1">
         <v>5</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1">
+      <c r="N8" s="1"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1">
         <v>6</v>
       </c>
-      <c r="O8" s="4">
+      <c r="S8" s="4">
         <v>7</v>
       </c>
-      <c r="P8" s="4">
+      <c r="T8" s="4">
         <v>8</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="U8" s="4">
         <v>9</v>
       </c>
-      <c r="R8" s="1">
+      <c r="V8" s="1">
         <v>10</v>
       </c>
-      <c r="S8" s="5">
+      <c r="W8" s="5">
         <v>11</v>
       </c>
-      <c r="T8" s="5">
+      <c r="X8" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="2"/>
       <c r="C9" s="4"/>
@@ -821,29 +878,33 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="X5:X7"/>
+    <mergeCell ref="A1:X2"/>
+    <mergeCell ref="S5:S7"/>
+    <mergeCell ref="T5:T7"/>
+    <mergeCell ref="U5:U7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="R5:R7"/>
+    <mergeCell ref="V5:V7"/>
+    <mergeCell ref="W5:W7"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="C4:X4"/>
+    <mergeCell ref="E6:J6"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="C5:C7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="T5:T7"/>
-    <mergeCell ref="A1:T2"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P5:P7"/>
-    <mergeCell ref="Q5:Q7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="N5:N7"/>
-    <mergeCell ref="R5:R7"/>
-    <mergeCell ref="S5:S7"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="C4:T4"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:Q6"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="88" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>

</xml_diff>